<commit_message>
Automatization of environmental accounts merging
</commit_message>
<xml_diff>
--- a/data/NRCan/Principal Mineral Areas, Producing Mines, and Oil and Gas Fields (900A)/metal_work.xlsx
+++ b/data/NRCan/Principal Mineral Areas, Producing Mines, and Oil and Gas Fields (900A)/metal_work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polymtlca0-my.sharepoint.com/personal/marin_pellan_polymtlus_ca/Documents/Desktop/POST_DOC/Project/regionalized_lci_mineral/data/NRCan/Principal Mineral Areas, Producing Mines, and Oil and Gas Fields (900A)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_3D018D26ACC0B63B03E60421A4B3CA66619F1283" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCA49A91-E492-4E0C-A4F5-C0C71BD7C6C3}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_3D018D26ACC0B63B03E60421A4B3CA66619F1283" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F894C845-B8D1-46CF-BBE4-61F273289DBF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="900a_73rd_metalworks" sheetId="1" r:id="rId1"/>
@@ -872,6 +872,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1193,7 +1197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J49" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -1262,154 +1266,154 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>197</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>198</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>199</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>170</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>171</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M2">
-        <v>43.274999999999999</v>
+        <v>49.2562</v>
       </c>
       <c r="N2">
-        <v>-79.819000000000003</v>
+        <v>-68.149100000000004</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>198</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>199</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>170</v>
+        <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L3" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M3">
-        <v>42.8001</v>
+        <v>46.693899999999999</v>
       </c>
       <c r="N3">
-        <v>-80.093699999999998</v>
+        <v>-71.946700000000007</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>204</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>204</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>198</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>199</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>163</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>170</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>171</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L4" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M4">
-        <v>46.52055</v>
+        <v>46.381</v>
       </c>
       <c r="N4">
-        <v>-84.366640000000004</v>
+        <v>-72.385199999999998</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="C5" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="D5" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="E5" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F5" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="G5" t="s">
         <v>163</v>
@@ -1430,174 +1434,174 @@
         <v>81</v>
       </c>
       <c r="M5">
-        <v>43.269131999999999</v>
+        <v>46.52055</v>
       </c>
       <c r="N5">
-        <v>-79.805204000000003</v>
+        <v>-84.366640000000004</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>210</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>211</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>211</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>169</v>
       </c>
       <c r="G6" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>164</v>
       </c>
       <c r="I6" t="s">
-        <v>87</v>
+        <v>170</v>
       </c>
       <c r="J6" t="s">
-        <v>88</v>
+        <v>171</v>
       </c>
       <c r="K6" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="L6" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="M6">
-        <v>43.942900000000002</v>
+        <v>53.492783000000003</v>
       </c>
       <c r="N6">
-        <v>-78.294300000000007</v>
+        <v>-113.387962</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>213</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>215</v>
       </c>
       <c r="E7" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="F7" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="G7" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="H7" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="I7" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="J7" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="K7" t="s">
-        <v>32</v>
+        <v>216</v>
       </c>
       <c r="L7" t="s">
-        <v>33</v>
+        <v>217</v>
       </c>
       <c r="M7">
-        <v>46.045864999999999</v>
+        <v>45.261305999999998</v>
       </c>
       <c r="N7">
-        <v>-73.124998000000005</v>
+        <v>-66.064603000000005</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>245</v>
       </c>
       <c r="B8" t="s">
-        <v>173</v>
+        <v>245</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
       <c r="D8" t="s">
-        <v>175</v>
+        <v>215</v>
       </c>
       <c r="E8" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="F8" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="G8" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="H8" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="I8" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="J8" t="s">
-        <v>177</v>
+        <v>138</v>
       </c>
       <c r="K8" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L8" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="M8">
-        <v>46.045907</v>
+        <v>43.259377999999998</v>
       </c>
       <c r="N8">
-        <v>-73.138424000000001</v>
+        <v>-79.778036</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>222</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="C9" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="D9" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="F9" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="G9" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="H9" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="I9" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="J9" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="K9" t="s">
         <v>32</v>
@@ -1606,42 +1610,42 @@
         <v>33</v>
       </c>
       <c r="M9">
-        <v>45.837722999999997</v>
+        <v>45.396324</v>
       </c>
       <c r="N9">
-        <v>-73.249081000000004</v>
+        <v>-73.500867</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="B10" t="s">
-        <v>183</v>
+        <v>230</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="D10" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="E10" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="F10" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="G10" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="H10" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="I10" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="J10" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="K10" t="s">
         <v>32</v>
@@ -1650,130 +1654,130 @@
         <v>33</v>
       </c>
       <c r="M10">
-        <v>45.819938</v>
+        <v>45.666409999999999</v>
       </c>
       <c r="N10">
-        <v>-73.263267999999997</v>
+        <v>-73.644812999999999</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>184</v>
+        <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>184</v>
+        <v>219</v>
       </c>
       <c r="C11" t="s">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="D11" t="s">
-        <v>185</v>
+        <v>215</v>
       </c>
       <c r="E11" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="F11" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="G11" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="H11" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="I11" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="J11" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="K11" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L11" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M11">
-        <v>45.611899999999999</v>
+        <v>46.747889999999998</v>
       </c>
       <c r="N11">
-        <v>-74.704435000000004</v>
+        <v>-71.177734000000001</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>186</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
       <c r="D12" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="E12" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="F12" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="G12" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="H12" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="I12" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="J12" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="K12" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L12" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M12">
-        <v>43.86</v>
+        <v>45.630899999999997</v>
       </c>
       <c r="N12">
-        <v>-78.91</v>
+        <v>-73.552199999999999</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>231</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="C13" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
       <c r="D13" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E13" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="F13" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="G13" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="H13" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="I13" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="J13" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="K13" t="s">
         <v>81</v>
@@ -1782,68 +1786,68 @@
         <v>81</v>
       </c>
       <c r="M13">
-        <v>42.998265000000004</v>
+        <v>45.407485000000001</v>
       </c>
       <c r="N13">
-        <v>-79.235065000000006</v>
+        <v>-75.606363999999999</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="B14" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="C14" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="D14" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="E14" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="F14" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="G14" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="H14" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="I14" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="J14" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="K14" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L14" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M14">
-        <v>43.37</v>
+        <v>45.833159999999999</v>
       </c>
       <c r="N14">
-        <v>-80.28</v>
+        <v>-73.260948999999997</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
       <c r="C15" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D15" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E15" t="s">
         <v>168</v>
@@ -1864,30 +1868,30 @@
         <v>171</v>
       </c>
       <c r="K15" t="s">
-        <v>206</v>
+        <v>32</v>
       </c>
       <c r="L15" t="s">
-        <v>206</v>
+        <v>33</v>
       </c>
       <c r="M15">
-        <v>50.130273000000003</v>
+        <v>45.837722999999997</v>
       </c>
       <c r="N15">
-        <v>-96.893632999999994</v>
+        <v>-73.249081000000004</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="C16" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="D16" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="E16" t="s">
         <v>168</v>
@@ -1908,36 +1912,36 @@
         <v>171</v>
       </c>
       <c r="K16" t="s">
-        <v>209</v>
+        <v>32</v>
       </c>
       <c r="L16" t="s">
-        <v>209</v>
+        <v>33</v>
       </c>
       <c r="M16">
-        <v>50.515262999999997</v>
+        <v>45.819938</v>
       </c>
       <c r="N16">
-        <v>-104.62384299999999</v>
+        <v>-73.263267999999997</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>210</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s">
-        <v>210</v>
+        <v>158</v>
       </c>
       <c r="C17" t="s">
-        <v>211</v>
+        <v>159</v>
       </c>
       <c r="D17" t="s">
-        <v>211</v>
+        <v>160</v>
       </c>
       <c r="E17" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F17" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G17" t="s">
         <v>163</v>
@@ -1946,168 +1950,168 @@
         <v>164</v>
       </c>
       <c r="I17" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="J17" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K17" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="L17" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
       <c r="M17">
-        <v>53.492783000000003</v>
+        <v>50.032130000000002</v>
       </c>
       <c r="N17">
-        <v>-113.387962</v>
+        <v>-66.797531000000006</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>135</v>
+        <v>192</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>192</v>
       </c>
       <c r="C18" t="s">
-        <v>136</v>
+        <v>193</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>193</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>194</v>
       </c>
       <c r="F18" t="s">
-        <v>138</v>
+        <v>195</v>
       </c>
       <c r="G18" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="H18" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="I18" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="J18" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="K18" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L18" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="M18">
-        <v>48.412768999999997</v>
+        <v>43.269131999999999</v>
       </c>
       <c r="N18">
-        <v>-71.131238999999994</v>
+        <v>-79.805204000000003</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>139</v>
+        <v>77</v>
       </c>
       <c r="H19" t="s">
-        <v>140</v>
+        <v>78</v>
       </c>
       <c r="I19" t="s">
-        <v>147</v>
+        <v>79</v>
       </c>
       <c r="J19" t="s">
-        <v>147</v>
+        <v>80</v>
       </c>
       <c r="K19" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L19" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="M19">
-        <v>48.531737999999997</v>
+        <v>43.691065999999999</v>
       </c>
       <c r="N19">
-        <v>-71.158168000000003</v>
+        <v>-79.722125000000005</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="B20" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F20" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="G20" t="s">
-        <v>139</v>
+        <v>18</v>
       </c>
       <c r="H20" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="J20" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="K20" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="L20" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="M20">
-        <v>46.37</v>
+        <v>51.060021999999996</v>
       </c>
       <c r="N20">
-        <v>-72.39</v>
+        <v>-115.210061</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>256</v>
       </c>
       <c r="B21" t="s">
-        <v>154</v>
+        <v>257</v>
       </c>
       <c r="C21" t="s">
-        <v>155</v>
+        <v>258</v>
       </c>
       <c r="D21" t="s">
-        <v>155</v>
+        <v>258</v>
       </c>
       <c r="E21" t="s">
         <v>138</v>
@@ -2116,130 +2120,130 @@
         <v>138</v>
       </c>
       <c r="G21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I21" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="J21" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="K21" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="L21" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="M21">
-        <v>45.298042000000002</v>
+        <v>51.024189999999997</v>
       </c>
       <c r="N21">
-        <v>-75.562391000000005</v>
+        <v>-114.031993</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>212</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s">
-        <v>213</v>
+        <v>111</v>
       </c>
       <c r="C22" t="s">
-        <v>214</v>
+        <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>215</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="H22" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="I22" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="J22" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="K22" t="s">
-        <v>216</v>
+        <v>81</v>
       </c>
       <c r="L22" t="s">
-        <v>217</v>
+        <v>81</v>
       </c>
       <c r="M22">
-        <v>45.261305999999998</v>
+        <v>46.180895999999997</v>
       </c>
       <c r="N22">
-        <v>-66.064603000000005</v>
+        <v>-83.017246</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>218</v>
+        <v>82</v>
       </c>
       <c r="B23" t="s">
-        <v>219</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>214</v>
+        <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>215</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>84</v>
       </c>
       <c r="F23" t="s">
-        <v>138</v>
+        <v>85</v>
       </c>
       <c r="G23" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="H23" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="I23" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="J23" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="K23" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L23" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="M23">
-        <v>46.747889999999998</v>
+        <v>43.942900000000002</v>
       </c>
       <c r="N23">
-        <v>-71.177734000000001</v>
+        <v>-78.294300000000007</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>220</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s">
-        <v>220</v>
+        <v>135</v>
       </c>
       <c r="C24" t="s">
-        <v>221</v>
+        <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>221</v>
+        <v>137</v>
       </c>
       <c r="E24" t="s">
         <v>138</v>
@@ -2248,16 +2252,16 @@
         <v>138</v>
       </c>
       <c r="G24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H24" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I24" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="J24" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="K24" t="s">
         <v>32</v>
@@ -2266,68 +2270,68 @@
         <v>33</v>
       </c>
       <c r="M24">
-        <v>45.833159999999999</v>
+        <v>48.412768999999997</v>
       </c>
       <c r="N24">
-        <v>-73.260948999999997</v>
+        <v>-71.131238999999994</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="B25" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="C25" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D25" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E25" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="F25" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="G25" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="H25" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="I25" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="J25" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="K25" t="s">
-        <v>32</v>
+        <v>209</v>
       </c>
       <c r="L25" t="s">
-        <v>33</v>
+        <v>209</v>
       </c>
       <c r="M25">
-        <v>45.396324</v>
+        <v>50.515262999999997</v>
       </c>
       <c r="N25">
-        <v>-73.500867</v>
+        <v>-104.62384299999999</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="B26" t="s">
-        <v>225</v>
+        <v>255</v>
       </c>
       <c r="C26" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D26" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E26" t="s">
         <v>138</v>
@@ -2348,30 +2352,30 @@
         <v>138</v>
       </c>
       <c r="K26" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="L26" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="M26">
-        <v>45.630899999999997</v>
+        <v>53.588118999999999</v>
       </c>
       <c r="N26">
-        <v>-73.552199999999999</v>
+        <v>-113.274102</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="B27" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="C27" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="D27" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="E27" t="s">
         <v>138</v>
@@ -2392,30 +2396,30 @@
         <v>138</v>
       </c>
       <c r="K27" t="s">
-        <v>32</v>
+        <v>206</v>
       </c>
       <c r="L27" t="s">
-        <v>33</v>
+        <v>206</v>
       </c>
       <c r="M27">
-        <v>45.397641999999998</v>
+        <v>49.928603000000003</v>
       </c>
       <c r="N27">
-        <v>-73.604969999999994</v>
+        <v>-97.019187000000002</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="B28" t="s">
-        <v>230</v>
+        <v>259</v>
       </c>
       <c r="C28" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D28" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E28" t="s">
         <v>138</v>
@@ -2436,30 +2440,30 @@
         <v>138</v>
       </c>
       <c r="K28" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="L28" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="M28">
-        <v>45.666409999999999</v>
+        <v>51.001803000000002</v>
       </c>
       <c r="N28">
-        <v>-73.644812999999999</v>
+        <v>-114.03286900000001</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="B29" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="C29" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D29" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E29" t="s">
         <v>138</v>
@@ -2480,30 +2484,30 @@
         <v>138</v>
       </c>
       <c r="K29" t="s">
-        <v>81</v>
+        <v>209</v>
       </c>
       <c r="L29" t="s">
-        <v>81</v>
+        <v>209</v>
       </c>
       <c r="M29">
-        <v>45.407485000000001</v>
+        <v>50.525046000000003</v>
       </c>
       <c r="N29">
-        <v>-75.606363999999999</v>
+        <v>-104.639712</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="B30" t="s">
-        <v>234</v>
+        <v>149</v>
       </c>
       <c r="C30" t="s">
-        <v>235</v>
+        <v>150</v>
       </c>
       <c r="D30" t="s">
-        <v>235</v>
+        <v>150</v>
       </c>
       <c r="E30" t="s">
         <v>138</v>
@@ -2512,42 +2516,42 @@
         <v>138</v>
       </c>
       <c r="G30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H30" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I30" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="J30" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="K30" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L30" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M30">
-        <v>44.912967999999999</v>
+        <v>46.37</v>
       </c>
       <c r="N30">
-        <v>-76.063979000000003</v>
+        <v>-72.39</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="B31" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="C31" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D31" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E31" t="s">
         <v>138</v>
@@ -2568,16 +2572,16 @@
         <v>138</v>
       </c>
       <c r="K31" t="s">
-        <v>81</v>
+        <v>206</v>
       </c>
       <c r="L31" t="s">
-        <v>81</v>
+        <v>206</v>
       </c>
       <c r="M31">
-        <v>44.261499999999998</v>
+        <v>50.133771000000003</v>
       </c>
       <c r="N31">
-        <v>-76.512100000000004</v>
+        <v>-96.911165999999994</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -2626,34 +2630,34 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>242</v>
+        <v>201</v>
       </c>
       <c r="B33" t="s">
-        <v>243</v>
+        <v>202</v>
       </c>
       <c r="C33" t="s">
-        <v>244</v>
+        <v>188</v>
       </c>
       <c r="D33" t="s">
-        <v>244</v>
+        <v>188</v>
       </c>
       <c r="E33" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="F33" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="G33" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="H33" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="I33" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="J33" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="K33" t="s">
         <v>81</v>
@@ -2662,86 +2666,86 @@
         <v>81</v>
       </c>
       <c r="M33">
-        <v>43.736238999999998</v>
+        <v>43.37</v>
       </c>
       <c r="N33">
-        <v>-79.666841000000005</v>
+        <v>-80.28</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
       <c r="B34" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
       <c r="C34" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="D34" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="F34" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="G34" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="H34" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="I34" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="J34" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="K34" t="s">
-        <v>81</v>
+        <v>206</v>
       </c>
       <c r="L34" t="s">
-        <v>81</v>
+        <v>206</v>
       </c>
       <c r="M34">
-        <v>43.259377999999998</v>
+        <v>50.130273000000003</v>
       </c>
       <c r="N34">
-        <v>-79.778036</v>
+        <v>-96.893632999999994</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>246</v>
+        <v>186</v>
       </c>
       <c r="B35" t="s">
-        <v>247</v>
+        <v>187</v>
       </c>
       <c r="C35" t="s">
-        <v>244</v>
+        <v>188</v>
       </c>
       <c r="D35" t="s">
-        <v>244</v>
+        <v>188</v>
       </c>
       <c r="E35" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="F35" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="G35" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="H35" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="I35" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="J35" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="K35" t="s">
         <v>81</v>
@@ -2750,244 +2754,244 @@
         <v>81</v>
       </c>
       <c r="M35">
-        <v>43.260956999999998</v>
+        <v>43.86</v>
       </c>
       <c r="N35">
-        <v>-79.782925000000006</v>
+        <v>-78.91</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>248</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>249</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>244</v>
+        <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>244</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
       <c r="F36" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="G36" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="H36" t="s">
-        <v>138</v>
+        <v>19</v>
       </c>
       <c r="I36" t="s">
-        <v>138</v>
+        <v>69</v>
       </c>
       <c r="J36" t="s">
-        <v>138</v>
+        <v>70</v>
       </c>
       <c r="K36" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L36" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M36">
-        <v>46.524326000000002</v>
+        <v>45.228312000000003</v>
       </c>
       <c r="N36">
-        <v>-84.395601999999997</v>
+        <v>-74.097205000000002</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>250</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>251</v>
+        <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>241</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>241</v>
+        <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
       <c r="F37" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="G37" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>138</v>
+        <v>19</v>
       </c>
       <c r="I37" t="s">
-        <v>138</v>
+        <v>54</v>
       </c>
       <c r="J37" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
       <c r="K37" t="s">
-        <v>206</v>
+        <v>32</v>
       </c>
       <c r="L37" t="s">
-        <v>206</v>
+        <v>33</v>
       </c>
       <c r="M37">
-        <v>50.133771000000003</v>
+        <v>45.627518000000002</v>
       </c>
       <c r="N37">
-        <v>-96.911165999999994</v>
+        <v>-73.511778000000007</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>252</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>252</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s">
-        <v>208</v>
+        <v>53</v>
       </c>
       <c r="D38" t="s">
-        <v>208</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
       <c r="F38" t="s">
-        <v>138</v>
+        <v>66</v>
       </c>
       <c r="G38" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="H38" t="s">
-        <v>138</v>
+        <v>19</v>
       </c>
       <c r="I38" t="s">
-        <v>138</v>
+        <v>61</v>
       </c>
       <c r="J38" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="K38" t="s">
-        <v>206</v>
+        <v>32</v>
       </c>
       <c r="L38" t="s">
-        <v>206</v>
+        <v>33</v>
       </c>
       <c r="M38">
-        <v>49.928603000000003</v>
+        <v>45.448518</v>
       </c>
       <c r="N38">
-        <v>-97.019187000000002</v>
+        <v>-73.676344999999998</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>253</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>253</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>253</v>
+        <v>53</v>
       </c>
       <c r="D39" t="s">
-        <v>253</v>
+        <v>53</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>27</v>
       </c>
       <c r="F39" t="s">
-        <v>138</v>
+        <v>28</v>
       </c>
       <c r="G39" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="H39" t="s">
-        <v>138</v>
+        <v>19</v>
       </c>
       <c r="I39" t="s">
-        <v>138</v>
+        <v>72</v>
       </c>
       <c r="J39" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
       <c r="K39" t="s">
-        <v>206</v>
+        <v>32</v>
       </c>
       <c r="L39" t="s">
-        <v>206</v>
+        <v>33</v>
       </c>
       <c r="M39">
-        <v>49.888469999999998</v>
+        <v>48.253399999999999</v>
       </c>
       <c r="N39">
-        <v>-97.098231999999996</v>
+        <v>-79.015100000000004</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>254</v>
+        <v>100</v>
       </c>
       <c r="B40" t="s">
-        <v>254</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>208</v>
+        <v>53</v>
       </c>
       <c r="D40" t="s">
-        <v>208</v>
+        <v>53</v>
       </c>
       <c r="E40" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="F40" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="G40" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="H40" t="s">
-        <v>138</v>
+        <v>19</v>
       </c>
       <c r="I40" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="J40" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="K40" t="s">
-        <v>209</v>
+        <v>81</v>
       </c>
       <c r="L40" t="s">
-        <v>209</v>
+        <v>81</v>
       </c>
       <c r="M40">
-        <v>50.525046000000003</v>
+        <v>46.576300000000003</v>
       </c>
       <c r="N40">
-        <v>-104.639712</v>
+        <v>-80.799300000000002</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="B41" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="C41" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="D41" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="E41" t="s">
         <v>138</v>
@@ -3008,74 +3012,74 @@
         <v>138</v>
       </c>
       <c r="K41" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="L41" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="M41">
-        <v>53.588118999999999</v>
+        <v>44.912967999999999</v>
       </c>
       <c r="N41">
-        <v>-113.274102</v>
+        <v>-76.063979000000003</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>256</v>
+        <v>184</v>
       </c>
       <c r="B42" t="s">
-        <v>257</v>
+        <v>184</v>
       </c>
       <c r="C42" t="s">
-        <v>258</v>
+        <v>185</v>
       </c>
       <c r="D42" t="s">
-        <v>258</v>
+        <v>185</v>
       </c>
       <c r="E42" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="F42" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="G42" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="H42" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="I42" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="J42" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="K42" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="L42" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="M42">
-        <v>51.024189999999997</v>
+        <v>45.611899999999999</v>
       </c>
       <c r="N42">
-        <v>-114.031993</v>
+        <v>-74.704435000000004</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B43" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C43" t="s">
-        <v>208</v>
+        <v>253</v>
       </c>
       <c r="D43" t="s">
-        <v>208</v>
+        <v>253</v>
       </c>
       <c r="E43" t="s">
         <v>138</v>
@@ -3096,30 +3100,30 @@
         <v>138</v>
       </c>
       <c r="K43" t="s">
-        <v>119</v>
+        <v>206</v>
       </c>
       <c r="L43" t="s">
-        <v>119</v>
+        <v>206</v>
       </c>
       <c r="M43">
-        <v>51.001803000000002</v>
+        <v>49.888469999999998</v>
       </c>
       <c r="N43">
-        <v>-114.03286900000001</v>
+        <v>-97.098231999999996</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>132</v>
+        <v>236</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>237</v>
       </c>
       <c r="C44" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
       <c r="D44" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
       <c r="E44" t="s">
         <v>138</v>
@@ -3140,30 +3144,30 @@
         <v>138</v>
       </c>
       <c r="K44" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="L44" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="M44">
-        <v>49.201528000000003</v>
+        <v>44.261499999999998</v>
       </c>
       <c r="N44">
-        <v>-123.086842</v>
+        <v>-76.512100000000004</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>261</v>
+        <v>143</v>
       </c>
       <c r="B45" t="s">
-        <v>262</v>
+        <v>144</v>
       </c>
       <c r="C45" t="s">
-        <v>263</v>
+        <v>145</v>
       </c>
       <c r="D45" t="s">
-        <v>263</v>
+        <v>146</v>
       </c>
       <c r="E45" t="s">
         <v>138</v>
@@ -3172,92 +3176,92 @@
         <v>138</v>
       </c>
       <c r="G45" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H45" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I45" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="J45" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="K45" t="s">
-        <v>130</v>
+        <v>32</v>
       </c>
       <c r="L45" t="s">
-        <v>131</v>
+        <v>33</v>
       </c>
       <c r="M45">
-        <v>48.43732</v>
+        <v>48.531737999999997</v>
       </c>
       <c r="N45">
-        <v>-123.37692</v>
+        <v>-71.158168000000003</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B46" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D46" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E46" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="F46" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="G46" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="H46" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="I46" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="J46" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="K46" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L46" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="M46">
-        <v>50.032130000000002</v>
+        <v>45.298042000000002</v>
       </c>
       <c r="N46">
-        <v>-66.797531000000006</v>
+        <v>-75.562391000000005</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B47" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C47" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="D47" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="E47" t="s">
-        <v>122</v>
+        <v>65</v>
       </c>
       <c r="F47" t="s">
-        <v>123</v>
+        <v>66</v>
       </c>
       <c r="G47" t="s">
         <v>18</v>
@@ -3266,186 +3270,186 @@
         <v>19</v>
       </c>
       <c r="I47" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="J47" t="s">
-        <v>125</v>
+        <v>62</v>
       </c>
       <c r="K47" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="L47" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="M47">
-        <v>51.060021999999996</v>
+        <v>49.194195999999998</v>
       </c>
       <c r="N47">
-        <v>-115.210061</v>
+        <v>-123.092001</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>261</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>262</v>
       </c>
       <c r="C48" t="s">
-        <v>15</v>
+        <v>263</v>
       </c>
       <c r="D48" t="s">
-        <v>15</v>
+        <v>263</v>
       </c>
       <c r="E48" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="F48" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
       <c r="G48" t="s">
-        <v>18</v>
+        <v>138</v>
       </c>
       <c r="H48" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="I48" t="s">
-        <v>20</v>
+        <v>138</v>
       </c>
       <c r="J48" t="s">
-        <v>21</v>
+        <v>138</v>
       </c>
       <c r="K48" t="s">
-        <v>22</v>
+        <v>130</v>
       </c>
       <c r="L48" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
       <c r="M48">
-        <v>47.410938000000002</v>
+        <v>48.43732</v>
       </c>
       <c r="N48">
-        <v>-53.811791999999997</v>
+        <v>-123.37692</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="D49" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="E49" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="F49" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="G49" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H49" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I49" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="J49" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="K49" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L49" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="M49">
-        <v>48.428476000000003</v>
+        <v>43.705800000000004</v>
       </c>
       <c r="N49">
-        <v>-71.157919000000007</v>
+        <v>-79.667100000000005</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C50" t="s">
-        <v>53</v>
+        <v>260</v>
       </c>
       <c r="D50" t="s">
-        <v>53</v>
+        <v>260</v>
       </c>
       <c r="E50" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="F50" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
       <c r="G50" t="s">
-        <v>18</v>
+        <v>138</v>
       </c>
       <c r="H50" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="I50" t="s">
-        <v>54</v>
+        <v>138</v>
       </c>
       <c r="J50" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="K50" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="L50" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="M50">
-        <v>45.627518000000002</v>
+        <v>49.201528000000003</v>
       </c>
       <c r="N50">
-        <v>-73.511778000000007</v>
+        <v>-123.086842</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D51" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E51" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F51" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G51" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H51" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I51" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="J51" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="K51" t="s">
         <v>32</v>
@@ -3454,200 +3458,200 @@
         <v>33</v>
       </c>
       <c r="M51">
-        <v>45.228312000000003</v>
+        <v>48.584699999999998</v>
       </c>
       <c r="N51">
-        <v>-74.097205000000002</v>
+        <v>-71.689700000000002</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="C52" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="D52" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="E52" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F52" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G52" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="H52" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="I52" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="J52" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="K52" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L52" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M52">
-        <v>45.431331999999998</v>
+        <v>48.430174000000001</v>
       </c>
       <c r="N52">
-        <v>-75.699219999999997</v>
+        <v>-71.165520999999998</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="B53" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C53" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="D53" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="E53" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F53" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G53" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H53" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I53" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="J53" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="K53" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L53" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M53">
-        <v>42.883000000000003</v>
+        <v>48.305799999999998</v>
       </c>
       <c r="N53">
-        <v>-79.239999999999995</v>
+        <v>-70.925799999999995</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="B54" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="D54" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="E54" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F54" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G54" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="H54" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="I54" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
       <c r="J54" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="K54" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="L54" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="M54">
-        <v>43.691065999999999</v>
+        <v>53.997599999999998</v>
       </c>
       <c r="N54">
-        <v>-79.722125000000005</v>
+        <v>-128.69540000000001</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="D55" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="E55" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F55" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G55" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="H55" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="I55" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="J55" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="K55" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L55" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M55">
-        <v>46.180895999999997</v>
+        <v>48.301299999999998</v>
       </c>
       <c r="N55">
-        <v>-83.017246</v>
+        <v>-71.128699999999995</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="B56" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="D56" t="s">
-        <v>116</v>
+        <v>39</v>
       </c>
       <c r="E56" t="s">
         <v>16</v>
@@ -3656,60 +3660,60 @@
         <v>17</v>
       </c>
       <c r="G56" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H56" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I56" t="s">
-        <v>117</v>
+        <v>42</v>
       </c>
       <c r="J56" t="s">
-        <v>118</v>
+        <v>43</v>
       </c>
       <c r="K56" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="L56" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
       <c r="M56">
-        <v>53.719929</v>
+        <v>48.428476000000003</v>
       </c>
       <c r="N56">
-        <v>-113.19011</v>
+        <v>-71.157919000000007</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="C57" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="D57" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="E57" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="F57" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="G57" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H57" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I57" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="J57" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="K57" t="s">
         <v>32</v>
@@ -3718,42 +3722,42 @@
         <v>33</v>
       </c>
       <c r="M57">
-        <v>45.402369</v>
+        <v>50.1571</v>
       </c>
       <c r="N57">
-        <v>-73.601868999999994</v>
+        <v>-66.442899999999995</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>172</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="C58" t="s">
-        <v>53</v>
+        <v>174</v>
       </c>
       <c r="D58" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="E58" t="s">
-        <v>65</v>
+        <v>168</v>
       </c>
       <c r="F58" t="s">
-        <v>66</v>
+        <v>169</v>
       </c>
       <c r="G58" t="s">
-        <v>18</v>
+        <v>163</v>
       </c>
       <c r="H58" t="s">
-        <v>19</v>
+        <v>164</v>
       </c>
       <c r="I58" t="s">
-        <v>61</v>
+        <v>176</v>
       </c>
       <c r="J58" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="K58" t="s">
         <v>32</v>
@@ -3762,86 +3766,86 @@
         <v>33</v>
       </c>
       <c r="M58">
-        <v>45.448518</v>
+        <v>46.045907</v>
       </c>
       <c r="N58">
-        <v>-73.676344999999998</v>
+        <v>-73.138424000000001</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>226</v>
       </c>
       <c r="B59" t="s">
-        <v>94</v>
+        <v>226</v>
       </c>
       <c r="C59" t="s">
-        <v>57</v>
+        <v>227</v>
       </c>
       <c r="D59" t="s">
-        <v>58</v>
+        <v>228</v>
       </c>
       <c r="E59" t="s">
-        <v>65</v>
+        <v>138</v>
       </c>
       <c r="F59" t="s">
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="G59" t="s">
-        <v>18</v>
+        <v>138</v>
       </c>
       <c r="H59" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="I59" t="s">
-        <v>61</v>
+        <v>138</v>
       </c>
       <c r="J59" t="s">
-        <v>62</v>
+        <v>138</v>
       </c>
       <c r="K59" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="L59" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M59">
-        <v>43.605060000000002</v>
+        <v>45.397641999999998</v>
       </c>
       <c r="N59">
-        <v>-79.579790000000003</v>
+        <v>-73.604969999999994</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C60" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="D60" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="E60" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="F60" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="G60" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="H60" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="I60" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="J60" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="K60" t="s">
         <v>81</v>
@@ -3850,30 +3854,30 @@
         <v>81</v>
       </c>
       <c r="M60">
-        <v>43.705800000000004</v>
+        <v>45.431331999999998</v>
       </c>
       <c r="N60">
-        <v>-79.667100000000005</v>
+        <v>-75.699219999999997</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B61" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="C61" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="D61" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="E61" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="F61" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="G61" t="s">
         <v>18</v>
@@ -3882,142 +3886,142 @@
         <v>19</v>
       </c>
       <c r="I61" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="J61" t="s">
-        <v>62</v>
+        <v>118</v>
       </c>
       <c r="K61" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="L61" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="M61">
-        <v>49.194195999999998</v>
+        <v>53.719929</v>
       </c>
       <c r="N61">
-        <v>-123.092001</v>
+        <v>-113.19011</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>24</v>
+        <v>196</v>
       </c>
       <c r="B62" t="s">
-        <v>24</v>
+        <v>196</v>
       </c>
       <c r="C62" t="s">
-        <v>25</v>
+        <v>197</v>
       </c>
       <c r="D62" t="s">
-        <v>26</v>
+        <v>197</v>
       </c>
       <c r="E62" t="s">
-        <v>27</v>
+        <v>198</v>
       </c>
       <c r="F62" t="s">
-        <v>28</v>
+        <v>199</v>
       </c>
       <c r="G62" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="H62" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="I62" t="s">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="J62" t="s">
-        <v>31</v>
+        <v>171</v>
       </c>
       <c r="K62" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L62" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="M62">
-        <v>50.1571</v>
+        <v>43.274999999999999</v>
       </c>
       <c r="N62">
-        <v>-66.442899999999995</v>
+        <v>-79.819000000000003</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>34</v>
+        <v>200</v>
       </c>
       <c r="B63" t="s">
-        <v>34</v>
+        <v>200</v>
       </c>
       <c r="C63" t="s">
-        <v>35</v>
+        <v>197</v>
       </c>
       <c r="D63" t="s">
-        <v>35</v>
+        <v>197</v>
       </c>
       <c r="E63" t="s">
-        <v>27</v>
+        <v>198</v>
       </c>
       <c r="F63" t="s">
-        <v>28</v>
+        <v>199</v>
       </c>
       <c r="G63" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="H63" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="I63" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="J63" t="s">
-        <v>37</v>
+        <v>171</v>
       </c>
       <c r="K63" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L63" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="M63">
-        <v>49.2562</v>
+        <v>42.8001</v>
       </c>
       <c r="N63">
-        <v>-68.149100000000004</v>
+        <v>-80.093699999999998</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>38</v>
+        <v>165</v>
       </c>
       <c r="B64" t="s">
-        <v>38</v>
+        <v>166</v>
       </c>
       <c r="C64" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="D64" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="E64" t="s">
-        <v>27</v>
+        <v>168</v>
       </c>
       <c r="F64" t="s">
-        <v>28</v>
+        <v>169</v>
       </c>
       <c r="G64" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="H64" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="I64" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="J64" t="s">
-        <v>37</v>
+        <v>171</v>
       </c>
       <c r="K64" t="s">
         <v>32</v>
@@ -4026,130 +4030,130 @@
         <v>33</v>
       </c>
       <c r="M64">
-        <v>48.305799999999998</v>
+        <v>46.045864999999999</v>
       </c>
       <c r="N64">
-        <v>-70.925799999999995</v>
+        <v>-73.124998000000005</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>40</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>126</v>
       </c>
       <c r="C65" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="D65" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="E65" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="F65" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="G65" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H65" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I65" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="J65" t="s">
-        <v>37</v>
+        <v>129</v>
       </c>
       <c r="K65" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="L65" t="s">
-        <v>33</v>
+        <v>131</v>
       </c>
       <c r="M65">
-        <v>48.301299999999998</v>
+        <v>49.099899999999998</v>
       </c>
       <c r="N65">
-        <v>-71.128699999999995</v>
+        <v>-117.7137</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="B66" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="C66" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D66" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="E66" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F66" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="G66" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H66" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I66" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="J66" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="K66" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L66" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="M66">
-        <v>48.430174000000001</v>
+        <v>43.605060000000002</v>
       </c>
       <c r="N66">
-        <v>-71.165520999999998</v>
+        <v>-79.579790000000003</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C67" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D67" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="E67" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="F67" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="G67" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H67" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="I67" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="J67" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="K67" t="s">
         <v>32</v>
@@ -4158,206 +4162,206 @@
         <v>33</v>
       </c>
       <c r="M67">
-        <v>48.584699999999998</v>
+        <v>45.402369</v>
       </c>
       <c r="N67">
-        <v>-71.689700000000002</v>
+        <v>-73.601868999999994</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>48</v>
+        <v>242</v>
       </c>
       <c r="B68" t="s">
-        <v>48</v>
+        <v>243</v>
       </c>
       <c r="C68" t="s">
-        <v>35</v>
+        <v>244</v>
       </c>
       <c r="D68" t="s">
-        <v>35</v>
+        <v>244</v>
       </c>
       <c r="E68" t="s">
-        <v>27</v>
+        <v>138</v>
       </c>
       <c r="F68" t="s">
-        <v>28</v>
+        <v>138</v>
       </c>
       <c r="G68" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="H68" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="I68" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
       <c r="J68" t="s">
-        <v>31</v>
+        <v>138</v>
       </c>
       <c r="K68" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L68" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="M68">
-        <v>46.693899999999999</v>
+        <v>43.736238999999998</v>
       </c>
       <c r="N68">
-        <v>-71.946700000000007</v>
+        <v>-79.666841000000005</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="B69" t="s">
-        <v>49</v>
+        <v>247</v>
       </c>
       <c r="C69" t="s">
-        <v>50</v>
+        <v>244</v>
       </c>
       <c r="D69" t="s">
-        <v>51</v>
+        <v>244</v>
       </c>
       <c r="E69" t="s">
-        <v>27</v>
+        <v>138</v>
       </c>
       <c r="F69" t="s">
-        <v>28</v>
+        <v>138</v>
       </c>
       <c r="G69" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="H69" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="I69" t="s">
-        <v>36</v>
+        <v>138</v>
       </c>
       <c r="J69" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="K69" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L69" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="M69">
-        <v>46.381</v>
+        <v>43.260956999999998</v>
       </c>
       <c r="N69">
-        <v>-72.385199999999998</v>
+        <v>-79.782925000000006</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>248</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>249</v>
       </c>
       <c r="C70" t="s">
-        <v>53</v>
+        <v>244</v>
       </c>
       <c r="D70" t="s">
-        <v>53</v>
+        <v>244</v>
       </c>
       <c r="E70" t="s">
-        <v>27</v>
+        <v>138</v>
       </c>
       <c r="F70" t="s">
-        <v>28</v>
+        <v>138</v>
       </c>
       <c r="G70" t="s">
-        <v>18</v>
+        <v>138</v>
       </c>
       <c r="H70" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="I70" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="J70" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
       <c r="K70" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="L70" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="M70">
-        <v>48.253399999999999</v>
+        <v>46.524326000000002</v>
       </c>
       <c r="N70">
-        <v>-79.015100000000004</v>
+        <v>-84.395601999999997</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>134</v>
+        <v>189</v>
       </c>
       <c r="B71" t="s">
-        <v>134</v>
+        <v>190</v>
       </c>
       <c r="C71" t="s">
-        <v>39</v>
+        <v>191</v>
       </c>
       <c r="D71" t="s">
-        <v>39</v>
+        <v>191</v>
       </c>
       <c r="E71" t="s">
-        <v>27</v>
+        <v>168</v>
       </c>
       <c r="F71" t="s">
-        <v>28</v>
+        <v>169</v>
       </c>
       <c r="G71" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="H71" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="I71" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="J71" t="s">
-        <v>37</v>
+        <v>171</v>
       </c>
       <c r="K71" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="L71" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="M71">
-        <v>53.997599999999998</v>
+        <v>42.998265000000004</v>
       </c>
       <c r="N71">
-        <v>-128.69540000000001</v>
+        <v>-79.235065000000006</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B72" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C72" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="D72" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="E72" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="F72" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="G72" t="s">
         <v>18</v>
@@ -4366,10 +4370,10 @@
         <v>19</v>
       </c>
       <c r="I72" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="J72" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="K72" t="s">
         <v>81</v>
@@ -4378,18 +4382,18 @@
         <v>81</v>
       </c>
       <c r="M72">
-        <v>46.576300000000003</v>
+        <v>46.4801</v>
       </c>
       <c r="N72">
-        <v>-80.799300000000002</v>
+        <v>-81.056899999999999</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B73" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C73" t="s">
         <v>90</v>
@@ -4398,10 +4402,10 @@
         <v>91</v>
       </c>
       <c r="E73" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="F73" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="G73" t="s">
         <v>18</v>
@@ -4410,10 +4414,10 @@
         <v>19</v>
       </c>
       <c r="I73" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="J73" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K73" t="s">
         <v>81</v>
@@ -4422,30 +4426,30 @@
         <v>81</v>
       </c>
       <c r="M73">
-        <v>46.4801</v>
+        <v>42.883000000000003</v>
       </c>
       <c r="N73">
-        <v>-81.056899999999999</v>
+        <v>-79.239999999999995</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>126</v>
+        <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>126</v>
+        <v>14</v>
       </c>
       <c r="C74" t="s">
-        <v>127</v>
+        <v>15</v>
       </c>
       <c r="D74" t="s">
-        <v>127</v>
+        <v>15</v>
       </c>
       <c r="E74" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="F74" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="G74" t="s">
         <v>18</v>
@@ -4454,28 +4458,28 @@
         <v>19</v>
       </c>
       <c r="I74" t="s">
-        <v>128</v>
+        <v>20</v>
       </c>
       <c r="J74" t="s">
-        <v>129</v>
+        <v>21</v>
       </c>
       <c r="K74" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="L74" t="s">
-        <v>131</v>
+        <v>23</v>
       </c>
       <c r="M74">
-        <v>49.099899999999998</v>
+        <v>47.410938000000002</v>
       </c>
       <c r="N74">
-        <v>-117.7137</v>
+        <v>-53.811791999999997</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N1" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N74">
-      <sortCondition ref="E1"/>
+      <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Progress on DB creation
</commit_message>
<xml_diff>
--- a/data/NRCan/Principal Mineral Areas, Producing Mines, and Oil and Gas Fields (900A)/metal_work.xlsx
+++ b/data/NRCan/Principal Mineral Areas, Producing Mines, and Oil and Gas Fields (900A)/metal_work.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="24" documentId="11_3D018D26ACC0B63B03E60421A4B3CA66619F1283" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F894C845-B8D1-46CF-BBE4-61F273289DBF}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2160" yWindow="2868" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="900a_73rd_metalworks" sheetId="1" r:id="rId1"/>
@@ -1198,7 +1198,7 @@
   <dimension ref="A1:N74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>